<commit_message>
NB finished, Halfway through methodologies
</commit_message>
<xml_diff>
--- a/Classifier1/Weighted_reduced.xlsx
+++ b/Classifier1/Weighted_reduced.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="18">
   <si>
     <t>DrugFamily</t>
   </si>
@@ -437,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,4 +2839,139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1">
+        <v>68</v>
+      </c>
+      <c r="F1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>138</v>
+      </c>
+      <c r="F3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>94</v>
+      </c>
+      <c r="F4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>138</v>
+      </c>
+      <c r="F6">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>